<commit_message>
spv see draft qpe dll
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/discipline-assesment (3).xlsx
+++ b/public/discipline-assesment/discipline-assesment (3).xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2C5485-8EB6-DA41-9439-30C27726303E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF364AC-89B1-5E40-9A9F-807E44E703BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -48,10 +56,10 @@
     <t>Terlambat</t>
   </si>
   <si>
-    <t>EN-4-070</t>
+    <t>KJ-6-168</t>
   </si>
   <si>
-    <t>Retno</t>
+    <t>Solihin</t>
   </si>
 </sst>
 </file>
@@ -70,14 +78,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -539,7 +547,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
notif email (disable for now)
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/discipline-assesment (3).xlsx
+++ b/public/discipline-assesment/discipline-assesment (3).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF364AC-89B1-5E40-9A9F-807E44E703BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9807040-29FD-8740-BD28-AB83A4E08CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,10 +56,10 @@
     <t>Terlambat</t>
   </si>
   <si>
-    <t>KJ-6-168</t>
+    <t>EN-4-072</t>
   </si>
   <si>
-    <t>Solihin</t>
+    <t>Agus C</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>